<commit_message>
Add Type column to Products export/import
- Add ItemType property to Product model for Product/Service distinction
- Update SpreadsheetExportService to include Type column in Products export
- Update SpreadsheetImportService to read Type column during Products import
- Update SampleCompanyData.xlsx with Type column in Products sheet
</commit_message>
<xml_diff>
--- a/SampleCompanyData.xlsx
+++ b/SampleCompanyData.xlsx
@@ -607,7 +607,6 @@
           <t>Thomas Miller</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
           <t>thomas.miller@email.com</t>
@@ -643,7 +642,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
           <t>Inactive</t>
@@ -704,7 +702,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr">
         <is>
           <t>Inactive</t>
@@ -765,7 +762,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
           <t>Active</t>
@@ -786,7 +782,6 @@
           <t>Sarah Williams</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
           <t>sarah.williams@email.com</t>
@@ -822,7 +817,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
           <t>Inactive</t>
@@ -908,7 +902,6 @@
           <t>David Hernandez</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
           <t>david.hernandez@email.com</t>
@@ -944,7 +937,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
           <t>Inactive</t>
@@ -965,7 +957,6 @@
           <t>Jane Johnson</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
           <t>jane.johnson@email.com</t>
@@ -1066,7 +1057,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr">
         <is>
           <t>Active</t>
@@ -1087,7 +1077,6 @@
           <t>John Rodriguez</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
           <t>john.rodriguez@email.com</t>
@@ -1123,7 +1112,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr">
         <is>
           <t>Active</t>
@@ -1184,7 +1172,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr">
         <is>
           <t>Active</t>
@@ -1205,7 +1192,6 @@
           <t>Barbara Jones</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
           <t>barbara.jones@email.com</t>
@@ -1306,7 +1292,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr">
         <is>
           <t>Active</t>
@@ -1327,7 +1312,6 @@
           <t>Maria Lopez</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr">
         <is>
           <t>maria.lopez@email.com</t>
@@ -1363,7 +1347,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr">
         <is>
           <t>Active</t>
@@ -1424,7 +1407,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr">
         <is>
           <t>Active</t>
@@ -1510,7 +1492,6 @@
           <t>Charles Jones</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
         <is>
           <t>charles.jones@email.com</t>
@@ -1546,7 +1527,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr">
         <is>
           <t>Active</t>
@@ -1607,7 +1587,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr">
         <is>
           <t>Active</t>
@@ -1668,7 +1647,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr">
         <is>
           <t>Active</t>
@@ -1689,7 +1667,6 @@
           <t>Jane Jones</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr">
         <is>
           <t>jane.jones@email.com</t>
@@ -1725,7 +1702,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr">
         <is>
           <t>Inactive</t>
@@ -7654,7 +7630,6 @@
           <t>2025-11-29</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
       <c r="H2" t="n">
         <v>293.05</v>
       </c>
@@ -7736,7 +7711,6 @@
           <t>2025-12-22</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr"/>
       <c r="H4" t="n">
         <v>366.97</v>
       </c>
@@ -7775,7 +7749,6 @@
           <t>2025-11-14</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr"/>
       <c r="H5" t="n">
         <v>288.98</v>
       </c>
@@ -7814,7 +7787,6 @@
           <t>2025-12-11</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
       <c r="H6" t="n">
         <v>157.83</v>
       </c>
@@ -7853,7 +7825,6 @@
           <t>2025-12-04</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr"/>
       <c r="H7" t="n">
         <v>63.3</v>
       </c>
@@ -7892,7 +7863,6 @@
           <t>2026-01-18</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr"/>
       <c r="H8" t="n">
         <v>276.14</v>
       </c>
@@ -7931,7 +7901,6 @@
           <t>2025-12-26</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr"/>
       <c r="H9" t="n">
         <v>254.3</v>
       </c>
@@ -8099,7 +8068,6 @@
           <t>2025-12-02</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr"/>
       <c r="H13" t="n">
         <v>338.25</v>
       </c>
@@ -8489,7 +8457,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -8542,7 +8509,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -8595,7 +8561,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -8648,7 +8613,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -8701,7 +8665,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -8754,7 +8717,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -8807,7 +8769,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -8860,7 +8821,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -8913,7 +8873,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -8966,7 +8925,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -9049,7 +9007,6 @@
           <t>Revenue</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
           <t>Electronic devices and accessories</t>
@@ -9193,7 +9150,6 @@
           <t>Revenue</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
           <t>General office supplies</t>
@@ -9226,7 +9182,6 @@
           <t>Revenue</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
           <t>Office and home furniture</t>
@@ -9259,7 +9214,6 @@
           <t>Revenue</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
           <t>Professional services</t>
@@ -9329,7 +9283,6 @@
           <t>Expenses</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
           <t>Manufacturing raw materials</t>
@@ -9362,7 +9315,6 @@
           <t>Expenses</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
           <t>Packaging materials</t>
@@ -9395,7 +9347,6 @@
           <t>Expenses</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr">
         <is>
           <t>Office-related purchases</t>
@@ -9428,7 +9379,6 @@
           <t>Expenses</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr">
         <is>
           <t>Utility expenses</t>
@@ -9461,7 +9411,6 @@
           <t>Expenses</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr">
         <is>
           <t>Marketing and advertising</t>
@@ -9494,7 +9443,6 @@
           <t>Expenses</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr">
         <is>
           <t>Software licenses and subscriptions</t>
@@ -9527,7 +9475,6 @@
           <t>Expenses</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr">
         <is>
           <t>Business equipment</t>
@@ -9555,7 +9502,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9582,22 +9529,27 @@
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>SKU</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Category ID</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Supplier ID</t>
         </is>
@@ -9616,20 +9568,25 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>LP15-2024</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>High-performance 15-inch laptop</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>CAT-SAL-002</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>SUP-004</t>
         </is>
@@ -9648,20 +9605,25 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>DW-X1</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>Professional desktop computer</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>CAT-SAL-002</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>SUP-004</t>
         </is>
@@ -9680,20 +9642,25 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>SPX12</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>Latest smartphone model</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>CAT-SAL-003</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>SUP-004</t>
         </is>
@@ -9712,20 +9679,25 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>TP-10</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>10-inch professional tablet</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>CAT-SAL-003</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>SUP-004</t>
         </is>
@@ -9744,20 +9716,25 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>WM-100</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>Ergonomic wireless mouse</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>CAT-SAL-004</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>SUP-002</t>
         </is>
@@ -9776,20 +9753,25 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>MK-RGB</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>RGB mechanical keyboard</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>CAT-SAL-004</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>SUP-002</t>
         </is>
@@ -9808,20 +9790,25 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t>USBC-7</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>7-port USB-C hub</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>CAT-SAL-004</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>SUP-002</t>
         </is>
@@ -9840,20 +9827,25 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
           <t>MON-27-4K</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>27-inch 4K monitor</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>CAT-SAL-001</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>SUP-004</t>
         </is>
@@ -9872,20 +9864,25 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
           <t>WC-1080</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>1080p HD webcam</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>CAT-SAL-004</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>SUP-002</t>
         </is>
@@ -9904,20 +9901,25 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
           <t>OC-ERG</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>Ergonomic office chair</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>CAT-SAL-006</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>SUP-003</t>
         </is>
@@ -9936,20 +9938,25 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
           <t>SD-ELEC</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>Electric standing desk</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>CAT-SAL-006</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>SUP-003</t>
         </is>
@@ -9968,20 +9975,25 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
           <t>FC-4DR</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>4-drawer filing cabinet</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>CAT-SAL-006</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>SUP-003</t>
         </is>
@@ -10000,20 +10012,25 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
           <t>PP-A4</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>A4 printer paper (500 sheets)</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>CAT-SAL-005</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>SUP-001</t>
         </is>
@@ -10032,20 +10049,25 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
           <t>IC-CLR</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>Color ink cartridge set</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>CAT-SAL-005</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>SUP-001</t>
         </is>
@@ -10064,20 +10086,25 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
           <t>ST-HD</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>Heavy-duty stapler</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>CAT-SAL-005</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>SUP-001</t>
         </is>
@@ -10096,20 +10123,25 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
           <t>NB-5PK</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>5-pack spiral notebooks</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>CAT-SAL-005</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="G17" t="inlineStr">
         <is>
           <t>SUP-001</t>
         </is>
@@ -10128,20 +10160,25 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
           <t>PN-12</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>12-pack ballpoint pens</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>CAT-SAL-005</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="G18" t="inlineStr">
         <is>
           <t>SUP-001</t>
         </is>
@@ -10160,20 +10197,25 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
           <t>DL-LED</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>LED desk lamp</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>CAT-SAL-005</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="G19" t="inlineStr">
         <is>
           <t>SUP-002</t>
         </is>
@@ -10192,20 +10234,25 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
           <t>CMK-10</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t>10-piece cable management kit</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="F20" t="inlineStr">
         <is>
           <t>CAT-SAL-004</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="G20" t="inlineStr">
         <is>
           <t>SUP-002</t>
         </is>
@@ -10224,20 +10271,25 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
           <t>SP-8OUT</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t>8-outlet surge protector</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="F21" t="inlineStr">
         <is>
           <t>CAT-SAL-004</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="G21" t="inlineStr">
         <is>
           <t>SUP-002</t>
         </is>
@@ -10256,20 +10308,25 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
           <t>SSD-1TB</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t>1TB external solid state drive</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="F22" t="inlineStr">
         <is>
           <t>CAT-SAL-004</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="G22" t="inlineStr">
         <is>
           <t>SUP-004</t>
         </is>
@@ -10288,20 +10345,25 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
           <t>HP-ANC</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t>Active noise cancelling headphones</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="F23" t="inlineStr">
         <is>
           <t>CAT-SAL-004</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="G23" t="inlineStr">
         <is>
           <t>SUP-004</t>
         </is>
@@ -10320,20 +10382,25 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
           <t>WB-48</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t>48-inch magnetic whiteboard</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
+      <c r="F24" t="inlineStr">
         <is>
           <t>CAT-SAL-005</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
+      <c r="G24" t="inlineStr">
         <is>
           <t>SUP-003</t>
         </is>
@@ -10352,20 +10419,25 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
           <t>DO-5C</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>5-compartment desk organizer</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
+      <c r="F25" t="inlineStr">
         <is>
           <t>CAT-SAL-005</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr">
+      <c r="G25" t="inlineStr">
         <is>
           <t>SUP-001</t>
         </is>
@@ -10384,20 +10456,25 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
           <t>MS-ADJ</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="E26" t="inlineStr">
         <is>
           <t>Adjustable monitor stand</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
+      <c r="F26" t="inlineStr">
         <is>
           <t>CAT-SAL-006</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr">
+      <c r="G26" t="inlineStr">
         <is>
           <t>SUP-003</t>
         </is>
@@ -13172,7 +13249,6 @@
           <t>REF-591283</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -13208,7 +13284,6 @@
           <t>REF-978578</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -13244,7 +13319,6 @@
           <t>REF-289796</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -13280,7 +13354,6 @@
           <t>REF-400031</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -13316,7 +13389,6 @@
           <t>REF-212997</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -13352,7 +13424,6 @@
           <t>REF-292091</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -13388,7 +13459,6 @@
           <t>REF-492050</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -13424,7 +13494,6 @@
           <t>REF-310408</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -13460,7 +13529,6 @@
           <t>REF-245200</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -13496,7 +13564,6 @@
           <t>REF-741176</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -13532,7 +13599,6 @@
           <t>REF-951472</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -13568,7 +13634,6 @@
           <t>REF-970342</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -13604,7 +13669,6 @@
           <t>REF-570690</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -13640,7 +13704,6 @@
           <t>REF-839814</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -13676,7 +13739,6 @@
           <t>REF-943892</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -13712,7 +13774,6 @@
           <t>REF-314959</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -13748,7 +13809,6 @@
           <t>REF-501296</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -13784,7 +13844,6 @@
           <t>REF-652963</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -13820,7 +13879,6 @@
           <t>REF-786875</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -13856,7 +13914,6 @@
           <t>REF-749895</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -13892,7 +13949,6 @@
           <t>REF-398987</t>
         </is>
       </c>
-      <c r="H22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -13928,7 +13984,6 @@
           <t>REF-949302</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -13964,7 +14019,6 @@
           <t>REF-632216</t>
         </is>
       </c>
-      <c r="H24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -14000,7 +14054,6 @@
           <t>REF-974781</t>
         </is>
       </c>
-      <c r="H25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -14036,7 +14089,6 @@
           <t>REF-287228</t>
         </is>
       </c>
-      <c r="H26" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add Type (Revenue/Expenses) and Item Type columns to Products
- Add CategoryType Type property to Product model for Revenue/Expenses/Rental
- Update export to include both Type and Item Type columns for Products
- Update import to read Type (Revenue/Expenses) and Item Type (Product/Service)
- Update SampleCompanyData.xlsx with both columns and proper header styling
</commit_message>
<xml_diff>
--- a/SampleCompanyData.xlsx
+++ b/SampleCompanyData.xlsx
@@ -45,7 +45,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -56,6 +56,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00D6EAF8"/>
         <bgColor rgb="00D6EAF8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ADD8E6"/>
+        <bgColor rgb="00ADD8E6"/>
       </patternFill>
     </fill>
   </fills>
@@ -71,9 +77,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -9502,7 +9511,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9529,27 +9538,32 @@
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Item Type</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>SKU</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Category ID</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Supplier ID</t>
         </is>
@@ -9568,25 +9582,30 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>LP15-2024</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>High-performance 15-inch laptop</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>CAT-SAL-002</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>SUP-004</t>
         </is>
@@ -9605,25 +9624,30 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>DW-X1</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>Professional desktop computer</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>CAT-SAL-002</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>SUP-004</t>
         </is>
@@ -9642,25 +9666,30 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>SPX12</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>Latest smartphone model</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>CAT-SAL-003</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>SUP-004</t>
         </is>
@@ -9679,25 +9708,30 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>TP-10</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>10-inch professional tablet</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>CAT-SAL-003</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>SUP-004</t>
         </is>
@@ -9716,25 +9750,30 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>WM-100</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>Ergonomic wireless mouse</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>CAT-SAL-004</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>SUP-002</t>
         </is>
@@ -9753,25 +9792,30 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>MK-RGB</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>RGB mechanical keyboard</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>CAT-SAL-004</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>SUP-002</t>
         </is>
@@ -9790,25 +9834,30 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>USBC-7</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>7-port USB-C hub</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>CAT-SAL-004</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>SUP-002</t>
         </is>
@@ -9827,25 +9876,30 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>MON-27-4K</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>27-inch 4K monitor</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>CAT-SAL-001</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>SUP-004</t>
         </is>
@@ -9864,25 +9918,30 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>WC-1080</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>1080p HD webcam</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>CAT-SAL-004</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>SUP-002</t>
         </is>
@@ -9901,25 +9960,30 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>OC-ERG</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>Ergonomic office chair</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>CAT-SAL-006</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>SUP-003</t>
         </is>
@@ -9938,25 +10002,30 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>SD-ELEC</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>Electric standing desk</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>CAT-SAL-006</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t>SUP-003</t>
         </is>
@@ -9975,25 +10044,30 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>FC-4DR</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>4-drawer filing cabinet</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>CAT-SAL-006</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t>SUP-003</t>
         </is>
@@ -10012,25 +10086,30 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>PP-A4</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>A4 printer paper (500 sheets)</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>CAT-SAL-005</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>SUP-001</t>
         </is>
@@ -10049,25 +10128,30 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>IC-CLR</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>Color ink cartridge set</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>CAT-SAL-005</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>SUP-001</t>
         </is>
@@ -10086,25 +10170,30 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>ST-HD</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>Heavy-duty stapler</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>CAT-SAL-005</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>SUP-001</t>
         </is>
@@ -10123,25 +10212,30 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>NB-5PK</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>5-pack spiral notebooks</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="G17" t="inlineStr">
         <is>
           <t>CAT-SAL-005</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="H17" t="inlineStr">
         <is>
           <t>SUP-001</t>
         </is>
@@ -10160,25 +10254,30 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>PN-12</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>12-pack ballpoint pens</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="G18" t="inlineStr">
         <is>
           <t>CAT-SAL-005</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="H18" t="inlineStr">
         <is>
           <t>SUP-001</t>
         </is>
@@ -10197,25 +10296,30 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>DL-LED</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>LED desk lamp</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="G19" t="inlineStr">
         <is>
           <t>CAT-SAL-005</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="H19" t="inlineStr">
         <is>
           <t>SUP-002</t>
         </is>
@@ -10234,25 +10338,30 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t>CMK-10</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="F20" t="inlineStr">
         <is>
           <t>10-piece cable management kit</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="G20" t="inlineStr">
         <is>
           <t>CAT-SAL-004</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="H20" t="inlineStr">
         <is>
           <t>SUP-002</t>
         </is>
@@ -10271,25 +10380,30 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t>SP-8OUT</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="F21" t="inlineStr">
         <is>
           <t>8-outlet surge protector</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="G21" t="inlineStr">
         <is>
           <t>CAT-SAL-004</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
+      <c r="H21" t="inlineStr">
         <is>
           <t>SUP-002</t>
         </is>
@@ -10308,25 +10422,30 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t>SSD-1TB</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="F22" t="inlineStr">
         <is>
           <t>1TB external solid state drive</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="G22" t="inlineStr">
         <is>
           <t>CAT-SAL-004</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
+      <c r="H22" t="inlineStr">
         <is>
           <t>SUP-004</t>
         </is>
@@ -10345,25 +10464,30 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t>HP-ANC</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="F23" t="inlineStr">
         <is>
           <t>Active noise cancelling headphones</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="G23" t="inlineStr">
         <is>
           <t>CAT-SAL-004</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
+      <c r="H23" t="inlineStr">
         <is>
           <t>SUP-004</t>
         </is>
@@ -10382,25 +10506,30 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t>WB-48</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
+      <c r="F24" t="inlineStr">
         <is>
           <t>48-inch magnetic whiteboard</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
+      <c r="G24" t="inlineStr">
         <is>
           <t>CAT-SAL-005</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr">
+      <c r="H24" t="inlineStr">
         <is>
           <t>SUP-003</t>
         </is>
@@ -10419,25 +10548,30 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>DO-5C</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
+      <c r="F25" t="inlineStr">
         <is>
           <t>5-compartment desk organizer</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr">
+      <c r="G25" t="inlineStr">
         <is>
           <t>CAT-SAL-005</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr">
+      <c r="H25" t="inlineStr">
         <is>
           <t>SUP-001</t>
         </is>
@@ -10456,25 +10590,30 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="E26" t="inlineStr">
         <is>
           <t>MS-ADJ</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
+      <c r="F26" t="inlineStr">
         <is>
           <t>Adjustable monitor stand</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr">
+      <c r="G26" t="inlineStr">
         <is>
           <t>CAT-SAL-006</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr">
+      <c r="H26" t="inlineStr">
         <is>
           <t>SUP-003</t>
         </is>

</xml_diff>

<commit_message>
Rename Description to Product in Expenses/Revenue sheets
- Rename Description column to Product in Expenses/Purchases export
- Rename Description column to Product in Revenue/Sales export
- Update imports to support both Product (new) and Description (legacy)
- Fix Type/Item Type header colors in xlsx to match other columns
- Add expense products to SampleCompanyData.xlsx Products sheet
</commit_message>
<xml_diff>
--- a/SampleCompanyData.xlsx
+++ b/SampleCompanyData.xlsx
@@ -1768,7 +1768,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Description</t>
+          <t>Product</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -3895,7 +3895,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Description</t>
+          <t>Product</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -9511,7 +9511,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9538,12 +9538,12 @@
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Item Type</t>
         </is>
@@ -10614,6 +10614,216 @@
         </is>
       </c>
       <c r="H26" t="inlineStr">
+        <is>
+          <t>SUP-003</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>PRD-026</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Office Supplies Bundle</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Expenses</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>OSB-001</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>General office supplies</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>CAT-PUR-001</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>SUP-001</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>PRD-027</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Printer Paper (Case)</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Expenses</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>PP-500</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>500 sheets per ream, 10 reams</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>CAT-PUR-001</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>SUP-001</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>PRD-028</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Cleaning Supplies Kit</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Expenses</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>CSK-001</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Commercial cleaning supplies</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>CAT-PUR-002</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>SUP-002</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>PRD-029</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>IT Support Service</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Expenses</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Service</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>ITS-HR</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Hourly IT support</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>CAT-PUR-003</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>SUP-004</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>PRD-030</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Marketing Consultation</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Expenses</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Service</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>MKT-HR</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Marketing consulting hourly</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>CAT-PUR-003</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
         <is>
           <t>SUP-003</t>
         </is>

</xml_diff>

<commit_message>
Fix product references in Expenses/Revenue sheets
Update SampleCompanyData.xlsx to use actual product names from the
Products sheet in Expenses and Revenue sheets instead of generic
descriptions that didn't exist as products.
</commit_message>
<xml_diff>
--- a/SampleCompanyData.xlsx
+++ b/SampleCompanyData.xlsx
@@ -1815,7 +1815,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Sale of electronics</t>
+          <t>Laptop Pro 15</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -1856,7 +1856,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Sale of consulting</t>
+          <t>IT Support Service</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -1897,7 +1897,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Sale of office supplies</t>
+          <t>Printer Paper</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Sale of electronics</t>
+          <t>Laptop Pro 15</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -1979,7 +1979,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Sale of office supplies</t>
+          <t>Printer Paper</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -2020,7 +2020,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Sale of furniture</t>
+          <t>Office Chair</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -2061,7 +2061,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Sale of electronics</t>
+          <t>Laptop Pro 15</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -2102,7 +2102,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Sale of electronics</t>
+          <t>Laptop Pro 15</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -2143,7 +2143,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Sale of consulting</t>
+          <t>IT Support Service</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -2184,7 +2184,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Sale of office supplies</t>
+          <t>Printer Paper</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -2225,7 +2225,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Sale of electronics</t>
+          <t>Laptop Pro 15</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -2266,7 +2266,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Sale of electronics</t>
+          <t>Laptop Pro 15</t>
         </is>
       </c>
       <c r="E13" t="n">
@@ -2307,7 +2307,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Sale of consulting</t>
+          <t>IT Support Service</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -2348,7 +2348,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Sale of electronics</t>
+          <t>Laptop Pro 15</t>
         </is>
       </c>
       <c r="E15" t="n">
@@ -2389,7 +2389,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Sale of electronics</t>
+          <t>Laptop Pro 15</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -2430,7 +2430,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Sale of electronics</t>
+          <t>Laptop Pro 15</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -2471,7 +2471,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Sale of office supplies</t>
+          <t>Printer Paper</t>
         </is>
       </c>
       <c r="E18" t="n">
@@ -2512,7 +2512,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Sale of consulting</t>
+          <t>IT Support Service</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -2553,7 +2553,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Sale of office supplies</t>
+          <t>Printer Paper</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -2594,7 +2594,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Sale of furniture</t>
+          <t>Office Chair</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -2635,7 +2635,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Sale of office supplies</t>
+          <t>Printer Paper</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -2676,7 +2676,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Sale of consulting</t>
+          <t>IT Support Service</t>
         </is>
       </c>
       <c r="E23" t="n">
@@ -2717,7 +2717,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Sale of electronics</t>
+          <t>Laptop Pro 15</t>
         </is>
       </c>
       <c r="E24" t="n">
@@ -2758,7 +2758,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Sale of office supplies</t>
+          <t>Printer Paper</t>
         </is>
       </c>
       <c r="E25" t="n">
@@ -2799,7 +2799,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Sale of electronics</t>
+          <t>Laptop Pro 15</t>
         </is>
       </c>
       <c r="E26" t="n">
@@ -2840,7 +2840,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Sale of office supplies</t>
+          <t>Printer Paper</t>
         </is>
       </c>
       <c r="E27" t="n">
@@ -2881,7 +2881,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Sale of electronics</t>
+          <t>Laptop Pro 15</t>
         </is>
       </c>
       <c r="E28" t="n">
@@ -2922,7 +2922,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Sale of consulting</t>
+          <t>IT Support Service</t>
         </is>
       </c>
       <c r="E29" t="n">
@@ -2963,7 +2963,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Sale of consulting</t>
+          <t>IT Support Service</t>
         </is>
       </c>
       <c r="E30" t="n">
@@ -3004,7 +3004,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Sale of consulting</t>
+          <t>IT Support Service</t>
         </is>
       </c>
       <c r="E31" t="n">
@@ -3045,7 +3045,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Sale of furniture</t>
+          <t>Office Chair</t>
         </is>
       </c>
       <c r="E32" t="n">
@@ -3086,7 +3086,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Sale of electronics</t>
+          <t>Laptop Pro 15</t>
         </is>
       </c>
       <c r="E33" t="n">
@@ -3127,7 +3127,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Sale of consulting</t>
+          <t>IT Support Service</t>
         </is>
       </c>
       <c r="E34" t="n">
@@ -3168,7 +3168,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Sale of electronics</t>
+          <t>Laptop Pro 15</t>
         </is>
       </c>
       <c r="E35" t="n">
@@ -3209,7 +3209,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Sale of electronics</t>
+          <t>Laptop Pro 15</t>
         </is>
       </c>
       <c r="E36" t="n">
@@ -3250,7 +3250,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Sale of services</t>
+          <t>Marketing Consultation</t>
         </is>
       </c>
       <c r="E37" t="n">
@@ -3291,7 +3291,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Sale of furniture</t>
+          <t>Office Chair</t>
         </is>
       </c>
       <c r="E38" t="n">
@@ -3332,7 +3332,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Sale of services</t>
+          <t>Marketing Consultation</t>
         </is>
       </c>
       <c r="E39" t="n">
@@ -3373,7 +3373,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Sale of furniture</t>
+          <t>Office Chair</t>
         </is>
       </c>
       <c r="E40" t="n">
@@ -3414,7 +3414,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Sale of electronics</t>
+          <t>Laptop Pro 15</t>
         </is>
       </c>
       <c r="E41" t="n">
@@ -3455,7 +3455,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Sale of furniture</t>
+          <t>Office Chair</t>
         </is>
       </c>
       <c r="E42" t="n">
@@ -3496,7 +3496,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Sale of services</t>
+          <t>Marketing Consultation</t>
         </is>
       </c>
       <c r="E43" t="n">
@@ -3537,7 +3537,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Sale of furniture</t>
+          <t>Office Chair</t>
         </is>
       </c>
       <c r="E44" t="n">
@@ -3578,7 +3578,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Sale of furniture</t>
+          <t>Office Chair</t>
         </is>
       </c>
       <c r="E45" t="n">
@@ -3619,7 +3619,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Sale of furniture</t>
+          <t>Office Chair</t>
         </is>
       </c>
       <c r="E46" t="n">
@@ -3660,7 +3660,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Sale of services</t>
+          <t>Marketing Consultation</t>
         </is>
       </c>
       <c r="E47" t="n">
@@ -3701,7 +3701,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Sale of services</t>
+          <t>Marketing Consultation</t>
         </is>
       </c>
       <c r="E48" t="n">
@@ -3742,7 +3742,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Sale of consulting</t>
+          <t>IT Support Service</t>
         </is>
       </c>
       <c r="E49" t="n">
@@ -3783,7 +3783,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Sale of consulting</t>
+          <t>IT Support Service</t>
         </is>
       </c>
       <c r="E50" t="n">
@@ -3824,7 +3824,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Sale of services</t>
+          <t>Marketing Consultation</t>
         </is>
       </c>
       <c r="E51" t="n">
@@ -3942,7 +3942,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Office supplies</t>
+          <t>Office Supplies Bundle</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -3983,7 +3983,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Office supplies</t>
+          <t>Office Supplies Bundle</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -4024,7 +4024,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Marketing materials</t>
+          <t>Marketing Consultation</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -4065,7 +4065,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Professional services</t>
+          <t>IT Support Service</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -4106,7 +4106,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Software subscription</t>
+          <t>IT Support Service</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -4147,7 +4147,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Equipment maintenance</t>
+          <t>Cleaning Supplies Kit</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -4188,7 +4188,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Marketing materials</t>
+          <t>Marketing Consultation</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -4229,7 +4229,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Professional services</t>
+          <t>IT Support Service</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -4270,7 +4270,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Software subscription</t>
+          <t>IT Support Service</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -4311,7 +4311,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Office supplies</t>
+          <t>Office Supplies Bundle</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -4352,7 +4352,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Office supplies</t>
+          <t>Office Supplies Bundle</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -4393,7 +4393,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Office supplies</t>
+          <t>Office Supplies Bundle</t>
         </is>
       </c>
       <c r="E13" t="n">
@@ -4434,7 +4434,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Office supplies</t>
+          <t>Office Supplies Bundle</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -4475,7 +4475,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Professional services</t>
+          <t>IT Support Service</t>
         </is>
       </c>
       <c r="E15" t="n">
@@ -4516,7 +4516,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Software subscription</t>
+          <t>IT Support Service</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -4557,7 +4557,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Marketing materials</t>
+          <t>Marketing Consultation</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -4598,7 +4598,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Utilities</t>
+          <t>Office Supplies Bundle</t>
         </is>
       </c>
       <c r="E18" t="n">
@@ -4639,7 +4639,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Travel expenses</t>
+          <t>Marketing Consultation</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -4680,7 +4680,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Utilities</t>
+          <t>Office Supplies Bundle</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -4721,7 +4721,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Utilities</t>
+          <t>Office Supplies Bundle</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -4762,7 +4762,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Equipment maintenance</t>
+          <t>Cleaning Supplies Kit</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -4803,7 +4803,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Equipment maintenance</t>
+          <t>Cleaning Supplies Kit</t>
         </is>
       </c>
       <c r="E23" t="n">
@@ -4844,7 +4844,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Equipment maintenance</t>
+          <t>Cleaning Supplies Kit</t>
         </is>
       </c>
       <c r="E24" t="n">
@@ -4885,7 +4885,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Office supplies</t>
+          <t>Office Supplies Bundle</t>
         </is>
       </c>
       <c r="E25" t="n">
@@ -4926,7 +4926,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Equipment maintenance</t>
+          <t>Cleaning Supplies Kit</t>
         </is>
       </c>
       <c r="E26" t="n">
@@ -4967,7 +4967,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Equipment maintenance</t>
+          <t>Cleaning Supplies Kit</t>
         </is>
       </c>
       <c r="E27" t="n">
@@ -5008,7 +5008,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Travel expenses</t>
+          <t>Marketing Consultation</t>
         </is>
       </c>
       <c r="E28" t="n">
@@ -5049,7 +5049,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Software subscription</t>
+          <t>IT Support Service</t>
         </is>
       </c>
       <c r="E29" t="n">
@@ -5090,7 +5090,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Office supplies</t>
+          <t>Office Supplies Bundle</t>
         </is>
       </c>
       <c r="E30" t="n">
@@ -5131,7 +5131,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Equipment maintenance</t>
+          <t>Cleaning Supplies Kit</t>
         </is>
       </c>
       <c r="E31" t="n">
@@ -5172,7 +5172,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Professional services</t>
+          <t>IT Support Service</t>
         </is>
       </c>
       <c r="E32" t="n">
@@ -5213,7 +5213,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Travel expenses</t>
+          <t>Marketing Consultation</t>
         </is>
       </c>
       <c r="E33" t="n">
@@ -5254,7 +5254,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Professional services</t>
+          <t>IT Support Service</t>
         </is>
       </c>
       <c r="E34" t="n">
@@ -5295,7 +5295,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Marketing materials</t>
+          <t>Marketing Consultation</t>
         </is>
       </c>
       <c r="E35" t="n">
@@ -5336,7 +5336,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Professional services</t>
+          <t>IT Support Service</t>
         </is>
       </c>
       <c r="E36" t="n">

</xml_diff>

<commit_message>
Remove 'Import Anyway' button and fix xlsx column widths
- Remove secondary "Import Anyway" button from missing references dialog
- User must now either create placeholders or cancel the import
- Widen Products sheet columns: Description, Category ID, Supplier ID
</commit_message>
<xml_diff>
--- a/SampleCompanyData.xlsx
+++ b/SampleCompanyData.xlsx
@@ -9520,11 +9520,13 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="9" customWidth="1" min="1" max="1"/>
-    <col width="22" customWidth="1" min="2" max="2"/>
+    <col width="25" customWidth="1" min="2" max="2"/>
     <col width="11" customWidth="1" min="3" max="3"/>
     <col width="36" customWidth="1" min="4" max="4"/>
     <col width="13" customWidth="1" min="5" max="5"/>
-    <col width="13" customWidth="1" min="6" max="6"/>
+    <col width="35" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="15" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>